<commit_message>
added EF Hutton ER
</commit_message>
<xml_diff>
--- a/ISSC/ISSC_Valuation_Model_20240522_v1.xlsx
+++ b/ISSC/ISSC_Valuation_Model_20240522_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewChen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewChen\Downloads\ISSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D99EA8-CA58-4BF4-8AC0-D22E637F1B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3CCE39-27CC-4B53-A084-13BA4C6DE1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{81AE2BAB-5DCF-4ACF-AB76-A5C9ECDD0E8C}"/>
   </bookViews>
@@ -214,12 +214,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.00_);\(0.00\)"/>
     <numFmt numFmtId="166" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +265,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -316,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -357,6 +364,8 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,8 +720,11 @@
   </sheetPr>
   <dimension ref="A2:BJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,104 +1620,104 @@
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="24">
         <f>3087.984-1038.847</f>
         <v>2049.1369999999997</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="24">
         <f>3685.702-1185.46</f>
         <v>2500.2420000000002</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="24">
         <f>3201.325-1000.436</f>
         <v>2200.8889999999997</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="24">
         <f>13450.803-SUM(C15:E15,C16:F16)</f>
         <v>2653.2700000000004</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="24">
         <f>3775.509-662.094</f>
         <v>3113.415</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="24">
         <f>3706.91-813.955</f>
         <v>2892.9549999999999</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="24">
         <f>4458.446-I16</f>
         <v>3398.9179999999997</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="24">
         <f>16165.333-SUM(G15:I15,G16:J16)</f>
         <v>3206.1259999999984</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="24">
         <f>4458.694-K16</f>
         <v>3269.6540000000005</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="24">
         <f>4645.682-1206.644</f>
         <v>3439.0379999999996</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="24">
         <f>5445.748-M16</f>
         <v>4539.0859999999993</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="24">
         <f>20806.121-SUM(K15:M15,K16:N16)</f>
         <v>5293.2569999999996</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="24">
         <f>4802.835-815.503</f>
         <v>3987.3319999999999</v>
       </c>
-      <c r="P15" s="17">
+      <c r="P15" s="24">
         <f>5102.67-1214.372</f>
         <v>3888.2979999999998</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="24">
         <f>5981.462-980.845</f>
         <v>5000.6170000000002</v>
       </c>
-      <c r="R15" s="17">
+      <c r="R15" s="24">
         <f>6873.116-1023.574</f>
         <v>5849.5420000000004</v>
       </c>
-      <c r="S15" s="17">
+      <c r="S15" s="24">
         <f>6695.778-1085.445</f>
         <v>5610.3330000000005</v>
       </c>
-      <c r="T15" s="17">
+      <c r="T15" s="24">
         <f>6647.617-1360.155</f>
         <v>5287.4620000000004</v>
       </c>
-      <c r="U15" s="17">
+      <c r="U15" s="24">
         <f>6935.976-1338.893</f>
         <v>5597.0829999999996</v>
       </c>
-      <c r="V15" s="17">
+      <c r="V15" s="24">
         <f>7000.379-1095.098</f>
         <v>5905.2809999999999</v>
       </c>
-      <c r="W15" s="17">
+      <c r="W15" s="24">
         <v>5088.2079999999996</v>
       </c>
-      <c r="X15" s="17">
+      <c r="X15" s="24">
         <v>5945.1509999999998</v>
       </c>
-      <c r="Y15" s="17">
+      <c r="Y15" s="24">
         <f>7893.625-1318.214</f>
         <v>6575.4110000000001</v>
       </c>
-      <c r="Z15" s="17">
+      <c r="Z15" s="24">
         <f>22589.657-SUM(W15:Y15)</f>
         <v>4980.8869999999988</v>
       </c>
-      <c r="AA15" s="17">
+      <c r="AA15" s="24">
         <v>4424.1080000000002</v>
       </c>
-      <c r="AB15" s="17">
+      <c r="AB15" s="24">
         <v>4895.5889999999999</v>
       </c>
     </row>
@@ -1713,88 +1725,88 @@
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="24">
         <v>1038.847</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="24">
         <v>1185.46</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="24">
         <v>1000.436</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="24">
         <f>4047.265-SUM(C16:E16)</f>
         <v>822.52199999999993</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="24">
         <v>662.09400000000005</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="24">
         <v>813.95500000000004</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="24">
         <v>1059.528</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="24">
         <f>3553.919-SUM(G16:I16)</f>
         <v>1018.3419999999996</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="24">
         <v>1189.04</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="24">
         <v>1206.644</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="24">
         <v>906.66200000000003</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="24">
         <f>4265.086-SUM(K16:M16)</f>
         <v>962.73999999999978</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="24">
         <v>815.50300000000004</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="24">
         <v>1214.3720000000001</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="24">
         <v>980.84500000000003</v>
       </c>
-      <c r="R16" s="17">
+      <c r="R16" s="24">
         <f>4034.294-SUM(O16:Q16)</f>
         <v>1023.5739999999996</v>
       </c>
-      <c r="S16" s="17">
+      <c r="S16" s="24">
         <v>1085.4449999999999</v>
       </c>
-      <c r="T16" s="17">
+      <c r="T16" s="24">
         <v>1360.155</v>
       </c>
-      <c r="U16" s="17">
+      <c r="U16" s="24">
         <v>1338.893</v>
       </c>
-      <c r="V16" s="17">
+      <c r="V16" s="24">
         <f>4879.591-SUM(S16:U16)</f>
         <v>1095.0980000000004</v>
       </c>
-      <c r="W16" s="17">
+      <c r="W16" s="24">
         <v>1061.1489999999999</v>
       </c>
-      <c r="X16" s="17">
+      <c r="X16" s="24">
         <v>1395.3030000000001</v>
       </c>
-      <c r="Y16" s="17">
+      <c r="Y16" s="24">
         <v>1318.2139999999999</v>
       </c>
-      <c r="Z16" s="17">
+      <c r="Z16" s="24">
         <f>11086.062-SUM(W16:Y16)</f>
         <v>7311.3959999999997</v>
       </c>
-      <c r="AA16" s="17">
+      <c r="AA16" s="24">
         <v>4227.2470000000003</v>
       </c>
-      <c r="AB16" s="17">
+      <c r="AB16" s="24">
         <v>5098.2219999999998</v>
       </c>
     </row>
@@ -1802,86 +1814,86 @@
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="17">
-        <v>0</v>
-      </c>
-      <c r="D17" s="17">
+      <c r="C17" s="24">
+        <v>0</v>
+      </c>
+      <c r="D17" s="24">
         <v>41.502000000000002</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="24">
         <v>188.33799999999999</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="24">
         <f>399.569-SUM(C17:E17)</f>
         <v>169.72900000000001</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="24">
         <v>202.14099999999999</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="24">
         <v>496.21699999999998</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="24">
         <v>131.37799999999999</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="24">
         <f>1407.256-SUM(G17:I17)</f>
         <v>577.52000000000021</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="24">
         <v>52.734000000000002</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="24">
         <v>189.38300000000001</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="24">
         <v>507.94099999999997</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17" s="24">
         <f>789.078-SUM(K17:M17)</f>
         <v>39.019999999999982</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17" s="24">
         <v>66.816999999999993</v>
       </c>
-      <c r="P17" s="17">
+      <c r="P17" s="24">
         <v>19.175000000000001</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="24">
         <v>198.721</v>
       </c>
-      <c r="R17" s="17">
-        <v>0</v>
-      </c>
-      <c r="S17" s="17">
-        <v>0</v>
-      </c>
-      <c r="T17" s="17">
+      <c r="R17" s="24">
+        <v>0</v>
+      </c>
+      <c r="S17" s="24">
+        <v>0</v>
+      </c>
+      <c r="T17" s="24">
         <v>198.203</v>
       </c>
-      <c r="U17" s="17">
-        <v>0</v>
-      </c>
-      <c r="V17" s="17">
+      <c r="U17" s="24">
+        <v>0</v>
+      </c>
+      <c r="V17" s="24">
         <v>262.74200000000002</v>
       </c>
-      <c r="W17" s="17">
+      <c r="W17" s="24">
         <v>366.899</v>
       </c>
-      <c r="X17" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="17">
+      <c r="X17" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="24">
         <v>65.582999999999998</v>
       </c>
-      <c r="Z17" s="17">
+      <c r="Z17" s="24">
         <f>1132.794-SUM(W17:Y17)</f>
         <v>700.31200000000013</v>
       </c>
-      <c r="AA17" s="17">
+      <c r="AA17" s="24">
         <v>656.70799999999997</v>
       </c>
-      <c r="AB17" s="17">
+      <c r="AB17" s="24">
         <v>745.70500000000004</v>
       </c>
     </row>
@@ -2194,104 +2206,104 @@
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="24">
         <f>1593.268-513.357</f>
         <v>1079.9110000000001</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="24">
         <f>2072.124-488.221</f>
         <v>1583.9029999999998</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="24">
         <f>1714.701-463.513</f>
         <v>1251.1880000000001</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="24">
         <f>7120.731-SUM(C21:E21,C22:F22)</f>
         <v>1481.5619999999999</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="24">
         <f>1723.281-325.152</f>
         <v>1398.1289999999999</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="24">
         <f>1567.861-303.813</f>
         <v>1264.0480000000002</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="24">
         <f>2009.799-353.348</f>
         <v>1656.451</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="24">
         <f>7038.717-SUM(G21:I21,G22:J22)</f>
         <v>1345.8619999999983</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="24">
         <f>1844.48-349.615</f>
         <v>1494.865</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="24">
         <f>2464.697-402.354</f>
         <v>2062.3430000000003</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="24">
         <f>2486.353-M22</f>
         <v>2165.9250000000002</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="24">
         <f>9568.553-SUM(K21:M21,K22:N22)</f>
         <v>2387.4249999999993</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="24">
         <f>2294.294-316.637</f>
         <v>1977.6569999999999</v>
       </c>
-      <c r="P21" s="17">
+      <c r="P21" s="24">
         <f>2211.649-354.664</f>
         <v>1856.9849999999999</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="24">
         <f>2764.765-408.161</f>
         <v>2356.6039999999998</v>
       </c>
-      <c r="R21" s="17">
+      <c r="R21" s="24">
         <f>2914.802-423.437</f>
         <v>2491.3650000000002</v>
       </c>
-      <c r="S21" s="17">
+      <c r="S21" s="24">
         <f>2728.057-343.65</f>
         <v>2384.4069999999997</v>
       </c>
-      <c r="T21" s="17">
+      <c r="T21" s="24">
         <f>2646.462-399.086</f>
         <v>2247.3760000000002</v>
       </c>
-      <c r="U21" s="17">
+      <c r="U21" s="24">
         <f>2879.462-369.562</f>
         <v>2509.9</v>
       </c>
-      <c r="V21" s="17">
+      <c r="V21" s="24">
         <f>2651.817-390.601</f>
         <v>2261.2159999999999</v>
       </c>
-      <c r="W21" s="17">
+      <c r="W21" s="24">
         <v>2415.944</v>
       </c>
-      <c r="X21" s="17">
+      <c r="X21" s="24">
         <v>2202.75</v>
       </c>
-      <c r="Y21" s="17">
+      <c r="Y21" s="24">
         <f>3202.87-371.359</f>
         <v>2831.511</v>
       </c>
-      <c r="Z21" s="17">
+      <c r="Z21" s="24">
         <f>9715.517-SUM(W21:Y21)</f>
         <v>2265.3119999999999</v>
       </c>
-      <c r="AA21" s="17">
+      <c r="AA21" s="24">
         <v>1781.345</v>
       </c>
-      <c r="AB21" s="17">
+      <c r="AB21" s="24">
         <v>2347.6950000000002</v>
       </c>
     </row>
@@ -2300,88 +2312,88 @@
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="24">
         <v>513.35699999999997</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="24">
         <v>488.221</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="24">
         <v>463.51299999999998</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="24">
         <f>1724.167-SUM(C22:E22)</f>
         <v>259.07600000000002</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="24">
         <v>325.15199999999999</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="24">
         <v>303.81299999999999</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I22" s="24">
         <v>353.34800000000001</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="24">
         <f>1374.227-SUM(G22:I22)</f>
         <v>391.91400000000021</v>
       </c>
-      <c r="K22" s="17">
+      <c r="K22" s="24">
         <v>349.61500000000001</v>
       </c>
-      <c r="L22" s="17">
+      <c r="L22" s="24">
         <v>402.35399999999998</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="24">
         <v>320.428</v>
       </c>
-      <c r="N22" s="17">
+      <c r="N22" s="24">
         <f>1457.995-SUM(K22:M22)</f>
         <v>385.59799999999996</v>
       </c>
-      <c r="O22" s="17">
+      <c r="O22" s="24">
         <v>316.637</v>
       </c>
-      <c r="P22" s="17">
+      <c r="P22" s="24">
         <v>354.66399999999999</v>
       </c>
-      <c r="Q22" s="17">
+      <c r="Q22" s="24">
         <v>408.161</v>
       </c>
-      <c r="R22" s="17">
+      <c r="R22" s="24">
         <f>1502.899-SUM(O22:Q22)</f>
         <v>423.4369999999999</v>
       </c>
-      <c r="S22" s="17">
+      <c r="S22" s="24">
         <v>343.65</v>
       </c>
-      <c r="T22" s="17">
+      <c r="T22" s="24">
         <v>399.08600000000001</v>
       </c>
-      <c r="U22" s="17">
+      <c r="U22" s="24">
         <v>369.56200000000001</v>
       </c>
-      <c r="V22" s="17">
+      <c r="V22" s="24">
         <f>1502.899-SUM(S22:U22)</f>
         <v>390.60099999999989</v>
       </c>
-      <c r="W22" s="17">
+      <c r="W22" s="24">
         <v>319.10199999999998</v>
       </c>
-      <c r="X22" s="17">
+      <c r="X22" s="24">
         <v>397.553</v>
       </c>
-      <c r="Y22" s="17">
+      <c r="Y22" s="24">
         <v>371.35899999999998</v>
       </c>
-      <c r="Z22" s="17">
+      <c r="Z22" s="24">
         <f>3386.122-SUM(W22:Y22)</f>
         <v>2298.1080000000002</v>
       </c>
-      <c r="AA22" s="17">
+      <c r="AA22" s="24">
         <v>1726.961</v>
       </c>
-      <c r="AB22" s="17">
+      <c r="AB22" s="24">
         <v>2462.2600000000002</v>
       </c>
     </row>
@@ -2390,87 +2402,87 @@
       <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="17">
-        <v>0</v>
-      </c>
-      <c r="D23" s="17">
+      <c r="C23" s="24">
+        <v>0</v>
+      </c>
+      <c r="D23" s="24">
         <v>10.223000000000001</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="24">
         <v>92.278999999999996</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="24">
         <f>191.192-SUM(C23:E23)</f>
         <v>88.690000000000012</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="24">
         <v>88.566000000000003</v>
       </c>
-      <c r="H23" s="17">
+      <c r="H23" s="24">
         <v>289.06</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="24">
         <v>54.817999999999998</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="24">
         <f>637.402-SUM(G23:I23)</f>
         <v>204.95800000000008</v>
       </c>
-      <c r="K23" s="17">
+      <c r="K23" s="24">
         <v>65.301000000000002</v>
       </c>
-      <c r="L23" s="17">
+      <c r="L23" s="24">
         <f>75.197</f>
         <v>75.197000000000003</v>
       </c>
-      <c r="M23" s="17">
+      <c r="M23" s="24">
         <v>72.662999999999997</v>
       </c>
-      <c r="N23" s="17">
+      <c r="N23" s="24">
         <f>224.671-SUM(K23:M23)</f>
         <v>11.509999999999991</v>
       </c>
-      <c r="O23" s="17">
+      <c r="O23" s="24">
         <v>9.5350000000000001</v>
       </c>
-      <c r="P23" s="17">
+      <c r="P23" s="24">
         <v>7.2050000000000001</v>
       </c>
-      <c r="Q23" s="17">
+      <c r="Q23" s="24">
         <v>60.915999999999997</v>
       </c>
-      <c r="R23" s="17">
-        <v>0</v>
-      </c>
-      <c r="S23" s="17">
-        <v>0</v>
-      </c>
-      <c r="T23" s="17">
+      <c r="R23" s="24">
+        <v>0</v>
+      </c>
+      <c r="S23" s="24">
+        <v>0</v>
+      </c>
+      <c r="T23" s="24">
         <v>16.748000000000001</v>
       </c>
-      <c r="U23" s="17">
-        <v>0</v>
-      </c>
-      <c r="V23" s="17">
+      <c r="U23" s="24">
+        <v>0</v>
+      </c>
+      <c r="V23" s="24">
         <v>143.768</v>
       </c>
-      <c r="W23" s="17">
+      <c r="W23" s="24">
         <v>57.405999999999999</v>
       </c>
-      <c r="X23" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="17">
+      <c r="X23" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="24">
         <v>21.692</v>
       </c>
-      <c r="Z23" s="17">
+      <c r="Z23" s="24">
         <f>395.803-SUM(W23:Y23)</f>
         <v>316.70499999999998</v>
       </c>
-      <c r="AA23" s="17">
+      <c r="AA23" s="24">
         <v>276.59500000000003</v>
       </c>
-      <c r="AB23" s="17">
+      <c r="AB23" s="24">
         <v>347.19900000000001</v>
       </c>
     </row>
@@ -3983,82 +3995,82 @@
       <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="24">
         <v>923.721</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="24">
         <v>1031.6220000000001</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="24">
         <v>1028.271</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="24">
         <v>592.18700000000001</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="24">
         <v>596.37199999999996</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H33" s="24">
         <v>648.48199999999997</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="24">
         <v>722.52499999999998</v>
       </c>
-      <c r="J33" s="17">
+      <c r="J33" s="24">
         <v>522.42700000000002</v>
       </c>
-      <c r="K33" s="17">
+      <c r="K33" s="24">
         <v>666.61500000000001</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="24">
         <v>712.01900000000001</v>
       </c>
-      <c r="M33" s="17">
+      <c r="M33" s="24">
         <v>870.80499999999995</v>
       </c>
-      <c r="N33" s="17">
+      <c r="N33" s="24">
         <v>706.53700000000003</v>
       </c>
-      <c r="O33" s="17">
+      <c r="O33" s="24">
         <v>600.298</v>
       </c>
-      <c r="P33" s="17">
+      <c r="P33" s="24">
         <v>689.654</v>
       </c>
-      <c r="Q33" s="17">
+      <c r="Q33" s="24">
         <v>646.79499999999996</v>
       </c>
-      <c r="R33" s="17">
+      <c r="R33" s="24">
         <v>686.17200000000003</v>
       </c>
-      <c r="S33" s="17">
+      <c r="S33" s="24">
         <v>736.52499999999998</v>
       </c>
-      <c r="T33" s="17">
+      <c r="T33" s="24">
         <v>650.03099999999995</v>
       </c>
-      <c r="U33" s="17">
+      <c r="U33" s="24">
         <v>676.38099999999997</v>
       </c>
-      <c r="V33" s="17">
+      <c r="V33" s="24">
         <v>642.20299999999997</v>
       </c>
-      <c r="W33" s="17">
+      <c r="W33" s="24">
         <v>670.44500000000005</v>
       </c>
-      <c r="X33" s="17">
+      <c r="X33" s="24">
         <v>866.19799999999998</v>
       </c>
-      <c r="Y33" s="17">
+      <c r="Y33" s="24">
         <v>851.29600000000005</v>
       </c>
-      <c r="Z33" s="17">
+      <c r="Z33" s="24">
         <v>741.57899999999995</v>
       </c>
-      <c r="AA33" s="17">
+      <c r="AA33" s="24">
         <v>901.14400000000001</v>
       </c>
-      <c r="AB33" s="17">
+      <c r="AB33" s="24">
         <v>1031.1189999999999</v>
       </c>
     </row>
@@ -4067,82 +4079,82 @@
       <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="24">
         <v>1622.5550000000001</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="24">
         <v>1756.7460000000001</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="24">
         <v>1626.64</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="24">
         <v>1668.2449999999999</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="24">
         <v>1473.4159999999999</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="24">
         <v>1524.6569999999999</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="24">
         <v>1416.0530000000001</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="24">
         <v>1463.7940000000001</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="24">
         <v>1703.2739999999999</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L34" s="24">
         <v>1531.3889999999999</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M34" s="24">
         <v>1279.422</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="24">
         <v>1586.461</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34" s="24">
         <v>1733.154</v>
       </c>
-      <c r="P34" s="17">
+      <c r="P34" s="24">
         <v>1602.1179999999999</v>
       </c>
-      <c r="Q34" s="17">
+      <c r="Q34" s="24">
         <v>1512.1379999999999</v>
       </c>
-      <c r="R34" s="17">
+      <c r="R34" s="24">
         <v>1410.3219999999999</v>
       </c>
-      <c r="S34" s="17">
+      <c r="S34" s="24">
         <v>1806.982</v>
       </c>
-      <c r="T34" s="17">
+      <c r="T34" s="24">
         <v>1724.8</v>
       </c>
-      <c r="U34" s="17">
+      <c r="U34" s="24">
         <v>1694.2329999999999</v>
       </c>
-      <c r="V34" s="17">
+      <c r="V34" s="24">
         <v>1527.9</v>
       </c>
-      <c r="W34" s="17">
+      <c r="W34" s="24">
         <v>2261.8629999999998</v>
       </c>
-      <c r="X34" s="17">
+      <c r="X34" s="24">
         <v>2446.6350000000002</v>
       </c>
-      <c r="Y34" s="17">
+      <c r="Y34" s="24">
         <v>2395.7139999999999</v>
       </c>
-      <c r="Z34" s="17">
+      <c r="Z34" s="24">
         <v>3718.2930000000001</v>
       </c>
-      <c r="AA34" s="17">
+      <c r="AA34" s="24">
         <v>3006.819</v>
       </c>
-      <c r="AB34" s="17">
+      <c r="AB34" s="24">
         <v>2908.1930000000002</v>
       </c>
     </row>
@@ -4887,82 +4899,82 @@
       <c r="B40" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="17">
-        <v>0</v>
-      </c>
-      <c r="D40" s="17">
-        <v>0</v>
-      </c>
-      <c r="E40" s="17">
-        <v>0</v>
-      </c>
-      <c r="F40" s="17">
-        <v>0</v>
-      </c>
-      <c r="G40" s="17">
-        <v>0</v>
-      </c>
-      <c r="H40" s="17">
-        <v>0</v>
-      </c>
-      <c r="I40" s="17">
-        <v>0</v>
-      </c>
-      <c r="J40" s="17">
-        <v>0</v>
-      </c>
-      <c r="K40" s="17">
-        <v>0</v>
-      </c>
-      <c r="L40" s="17">
-        <v>0</v>
-      </c>
-      <c r="M40" s="17">
-        <v>0</v>
-      </c>
-      <c r="N40" s="17">
-        <v>0</v>
-      </c>
-      <c r="O40" s="17">
-        <v>0</v>
-      </c>
-      <c r="P40" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="17">
-        <v>0</v>
-      </c>
-      <c r="R40" s="17">
-        <v>0</v>
-      </c>
-      <c r="S40" s="17">
-        <v>0</v>
-      </c>
-      <c r="T40" s="17">
-        <v>0</v>
-      </c>
-      <c r="U40" s="17">
-        <v>0</v>
-      </c>
-      <c r="V40" s="17">
-        <v>0</v>
-      </c>
-      <c r="W40" s="17">
-        <v>0</v>
-      </c>
-      <c r="X40" s="17">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="17">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="17">
+      <c r="C40" s="24">
+        <v>0</v>
+      </c>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
+      <c r="E40" s="24">
+        <v>0</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0</v>
+      </c>
+      <c r="I40" s="24">
+        <v>0</v>
+      </c>
+      <c r="J40" s="24">
+        <v>0</v>
+      </c>
+      <c r="K40" s="24">
+        <v>0</v>
+      </c>
+      <c r="L40" s="24">
+        <v>0</v>
+      </c>
+      <c r="M40" s="24">
+        <v>0</v>
+      </c>
+      <c r="N40" s="24">
+        <v>0</v>
+      </c>
+      <c r="O40" s="24">
+        <v>0</v>
+      </c>
+      <c r="P40" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="24">
+        <v>0</v>
+      </c>
+      <c r="R40" s="24">
+        <v>0</v>
+      </c>
+      <c r="S40" s="24">
+        <v>0</v>
+      </c>
+      <c r="T40" s="24">
+        <v>0</v>
+      </c>
+      <c r="U40" s="24">
+        <v>0</v>
+      </c>
+      <c r="V40" s="24">
+        <v>0</v>
+      </c>
+      <c r="W40" s="24">
+        <v>0</v>
+      </c>
+      <c r="X40" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="24">
         <v>-393.28100000000001</v>
       </c>
-      <c r="AA40" s="17">
+      <c r="AA40" s="24">
         <v>-360.01299999999998</v>
       </c>
-      <c r="AB40" s="17">
+      <c r="AB40" s="24">
         <v>-171.47</v>
       </c>
     </row>
@@ -4971,82 +4983,82 @@
       <c r="B41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="24">
         <v>9.6240000000000006</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="24">
         <v>11.680999999999999</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="24">
         <v>15.164</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="24">
         <v>17.091999999999999</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G41" s="24">
         <v>21.552</v>
       </c>
-      <c r="H41" s="17">
+      <c r="H41" s="24">
         <v>26.48</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I41" s="24">
         <v>99.915999999999997</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="24">
         <v>101.672</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K41" s="24">
         <v>78.87</v>
       </c>
-      <c r="L41" s="17">
+      <c r="L41" s="24">
         <v>65.721000000000004</v>
       </c>
-      <c r="M41" s="17">
+      <c r="M41" s="24">
         <v>7.7670000000000003</v>
       </c>
-      <c r="N41" s="17">
+      <c r="N41" s="24">
         <v>2.5920000000000001</v>
       </c>
-      <c r="O41" s="17">
+      <c r="O41" s="24">
         <v>0.879</v>
       </c>
-      <c r="P41" s="17">
+      <c r="P41" s="24">
         <v>0.152</v>
       </c>
-      <c r="Q41" s="17">
+      <c r="Q41" s="24">
         <v>0.107</v>
       </c>
-      <c r="R41" s="17">
+      <c r="R41" s="24">
         <v>23.911999999999999</v>
       </c>
-      <c r="S41" s="17">
+      <c r="S41" s="24">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="T41" s="17">
+      <c r="T41" s="24">
         <v>0.34599999999999997</v>
       </c>
-      <c r="U41" s="17">
+      <c r="U41" s="24">
         <v>10.429</v>
       </c>
-      <c r="V41" s="17">
+      <c r="V41" s="24">
         <v>65.231999999999999</v>
       </c>
-      <c r="W41" s="17">
+      <c r="W41" s="24">
         <v>115.892</v>
       </c>
-      <c r="X41" s="17">
+      <c r="X41" s="24">
         <v>130.95099999999999</v>
       </c>
-      <c r="Y41" s="17">
+      <c r="Y41" s="24">
         <v>185.65199999999999</v>
       </c>
-      <c r="Z41" s="17">
+      <c r="Z41" s="24">
         <v>85.692999999999998</v>
       </c>
-      <c r="AA41" s="17">
+      <c r="AA41" s="24">
         <v>79.478999999999999</v>
       </c>
-      <c r="AB41" s="17">
+      <c r="AB41" s="24">
         <v>36.200000000000003</v>
       </c>
     </row>
@@ -5055,82 +5067,82 @@
       <c r="B42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="24">
         <v>21.431000000000001</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="24">
         <v>15.664</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="24">
         <v>16.128</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="24">
         <v>14.5</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G42" s="24">
         <v>21.853999999999999</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H42" s="24">
         <v>10.746</v>
       </c>
-      <c r="I42" s="17">
+      <c r="I42" s="24">
         <v>24.713999999999999</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="24">
         <v>16.422999999999998</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K42" s="24">
         <v>17.28</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L42" s="24">
         <v>11.218999999999999</v>
       </c>
-      <c r="M42" s="17">
+      <c r="M42" s="24">
         <v>16.260999999999999</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N42" s="24">
         <v>15.737</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O42" s="24">
         <v>16.391999999999999</v>
       </c>
-      <c r="P42" s="17">
+      <c r="P42" s="24">
         <v>17.370999999999999</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q42" s="24">
         <v>17.231000000000002</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R42" s="24">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="S42" s="17">
+      <c r="S42" s="24">
         <v>16.238</v>
       </c>
-      <c r="T42" s="17">
+      <c r="T42" s="24">
         <v>11.555</v>
       </c>
-      <c r="U42" s="17">
+      <c r="U42" s="24">
         <v>21.608000000000001</v>
       </c>
-      <c r="V42" s="17">
+      <c r="V42" s="24">
         <v>50.179000000000002</v>
       </c>
-      <c r="W42" s="17">
+      <c r="W42" s="24">
         <v>18.196000000000002</v>
       </c>
-      <c r="X42" s="17">
+      <c r="X42" s="24">
         <v>23.257999999999999</v>
       </c>
-      <c r="Y42" s="17">
+      <c r="Y42" s="24">
         <v>90.049000000000007</v>
       </c>
-      <c r="Z42" s="17">
+      <c r="Z42" s="24">
         <v>19.812999999999999</v>
       </c>
-      <c r="AA42" s="17">
+      <c r="AA42" s="24">
         <v>17.699000000000002</v>
       </c>
-      <c r="AB42" s="17">
+      <c r="AB42" s="24">
         <v>26.472000000000001</v>
       </c>
     </row>
@@ -5780,6 +5792,110 @@
       <c r="B48" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C48" s="17">
+        <f>C40-C41</f>
+        <v>-9.6240000000000006</v>
+      </c>
+      <c r="D48" s="17">
+        <f t="shared" ref="D48:AB48" si="102">D40-D41</f>
+        <v>-11.680999999999999</v>
+      </c>
+      <c r="E48" s="17">
+        <f t="shared" si="102"/>
+        <v>-15.164</v>
+      </c>
+      <c r="F48" s="17">
+        <f t="shared" si="102"/>
+        <v>-17.091999999999999</v>
+      </c>
+      <c r="G48" s="17">
+        <f t="shared" si="102"/>
+        <v>-21.552</v>
+      </c>
+      <c r="H48" s="17">
+        <f t="shared" si="102"/>
+        <v>-26.48</v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="102"/>
+        <v>-99.915999999999997</v>
+      </c>
+      <c r="J48" s="17">
+        <f t="shared" si="102"/>
+        <v>-101.672</v>
+      </c>
+      <c r="K48" s="17">
+        <f t="shared" si="102"/>
+        <v>-78.87</v>
+      </c>
+      <c r="L48" s="17">
+        <f t="shared" si="102"/>
+        <v>-65.721000000000004</v>
+      </c>
+      <c r="M48" s="17">
+        <f t="shared" si="102"/>
+        <v>-7.7670000000000003</v>
+      </c>
+      <c r="N48" s="17">
+        <f t="shared" si="102"/>
+        <v>-2.5920000000000001</v>
+      </c>
+      <c r="O48" s="17">
+        <f t="shared" si="102"/>
+        <v>-0.879</v>
+      </c>
+      <c r="P48" s="17">
+        <f t="shared" si="102"/>
+        <v>-0.152</v>
+      </c>
+      <c r="Q48" s="17">
+        <f t="shared" si="102"/>
+        <v>-0.107</v>
+      </c>
+      <c r="R48" s="17">
+        <f t="shared" si="102"/>
+        <v>-23.911999999999999</v>
+      </c>
+      <c r="S48" s="17">
+        <f t="shared" si="102"/>
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="T48" s="17">
+        <f t="shared" si="102"/>
+        <v>-0.34599999999999997</v>
+      </c>
+      <c r="U48" s="17">
+        <f t="shared" si="102"/>
+        <v>-10.429</v>
+      </c>
+      <c r="V48" s="17">
+        <f t="shared" si="102"/>
+        <v>-65.231999999999999</v>
+      </c>
+      <c r="W48" s="17">
+        <f t="shared" si="102"/>
+        <v>-115.892</v>
+      </c>
+      <c r="X48" s="17">
+        <f t="shared" si="102"/>
+        <v>-130.95099999999999</v>
+      </c>
+      <c r="Y48" s="17">
+        <f t="shared" si="102"/>
+        <v>-185.65199999999999</v>
+      </c>
+      <c r="Z48" s="17">
+        <f t="shared" si="102"/>
+        <v>-478.97399999999999</v>
+      </c>
+      <c r="AA48" s="17">
+        <f t="shared" si="102"/>
+        <v>-439.49199999999996</v>
+      </c>
+      <c r="AB48" s="17">
+        <f t="shared" si="102"/>
+        <v>-207.67000000000002</v>
+      </c>
     </row>
     <row r="49" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
@@ -5791,240 +5907,104 @@
         <v>-138.886</v>
       </c>
       <c r="D49" s="17">
-        <f t="shared" ref="D49:BJ49" si="102">D45</f>
+        <f t="shared" ref="D49:AB49" si="103">D45</f>
         <v>200.70500000000001</v>
       </c>
       <c r="E49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>0.10100000000000001</v>
       </c>
       <c r="F49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>1.7310000000000001</v>
       </c>
       <c r="G49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
       <c r="H49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>7.7939999999999996</v>
       </c>
       <c r="I49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
       <c r="J49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>-5.9889999999999999</v>
       </c>
       <c r="K49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
       <c r="L49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>-309.40199999999999</v>
       </c>
       <c r="M49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>8.6159999999999997</v>
       </c>
       <c r="N49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>-8.0960000000000001</v>
       </c>
       <c r="O49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>9.4969999999999999</v>
       </c>
       <c r="P49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>20.164999999999999</v>
       </c>
       <c r="Q49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>-1473.0139999999999</v>
       </c>
       <c r="R49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>355.56900000000002</v>
       </c>
       <c r="S49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>307.49</v>
       </c>
       <c r="T49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>390.11</v>
       </c>
       <c r="U49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>358.76299999999998</v>
       </c>
       <c r="V49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>761.46799999999996</v>
       </c>
       <c r="W49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>226.93299999999999</v>
       </c>
       <c r="X49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>310.42399999999998</v>
       </c>
       <c r="Y49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>339.95800000000003</v>
       </c>
       <c r="Z49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>730.202</v>
       </c>
       <c r="AA49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>295.01400000000001</v>
       </c>
       <c r="AB49" s="17">
-        <f t="shared" si="102"/>
+        <f t="shared" si="103"/>
         <v>325.93599999999998</v>
-      </c>
-      <c r="AC49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AD49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AE49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AF49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AG49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AH49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AI49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AK49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AL49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AM49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AN49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AO49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AP49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AQ49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AR49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AS49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AT49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AU49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AV49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AW49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AX49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AY49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="AZ49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BA49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BB49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BC49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BD49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BE49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BF49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BG49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BH49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BI49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
-      </c>
-      <c r="BJ49" s="17">
-        <f t="shared" si="102"/>
-        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -6032,144 +6012,596 @@
       <c r="B50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="W50" s="17">
+      <c r="C50" s="25">
+        <v>103.36799999999999</v>
+      </c>
+      <c r="D50" s="25">
+        <f>210.549-C50</f>
+        <v>107.18100000000001</v>
+      </c>
+      <c r="E50" s="25">
+        <f>316.855-SUM(C50:D50)</f>
+        <v>106.30600000000001</v>
+      </c>
+      <c r="F50" s="25">
+        <f>436.208-SUM(C50:E50)</f>
+        <v>119.35300000000001</v>
+      </c>
+      <c r="G50" s="25">
+        <v>116.078</v>
+      </c>
+      <c r="H50" s="25">
+        <f>234.846-G50</f>
+        <v>118.768</v>
+      </c>
+      <c r="I50" s="25">
+        <f>342.359-SUM(G50:H50)</f>
+        <v>107.51299999999998</v>
+      </c>
+      <c r="J50" s="25">
+        <f>451.278-SUM(G50:I50)</f>
+        <v>108.91900000000004</v>
+      </c>
+      <c r="K50" s="25">
+        <f>104.135</f>
+        <v>104.13500000000001</v>
+      </c>
+      <c r="L50" s="25">
+        <f>205.154-K50</f>
+        <v>101.01899999999999</v>
+      </c>
+      <c r="M50" s="25">
+        <f>301.55-SUM(K50:L50)</f>
+        <v>96.396000000000015</v>
+      </c>
+      <c r="N50" s="25">
+        <f>433.51-SUM(K50:M50)</f>
+        <v>131.95999999999998</v>
+      </c>
+      <c r="O50" s="25">
+        <v>113.682</v>
+      </c>
+      <c r="P50" s="25">
+        <f>224.478-O50</f>
+        <v>110.79600000000001</v>
+      </c>
+      <c r="Q50" s="25">
+        <f>334.25-SUM(O50:P50)</f>
+        <v>109.77199999999999</v>
+      </c>
+      <c r="R50" s="25">
+        <f>432.176-SUM(O50:Q50)</f>
+        <v>97.925999999999988</v>
+      </c>
+      <c r="S50" s="25">
+        <v>92.372</v>
+      </c>
+      <c r="T50" s="25">
+        <f>188.136-S50</f>
+        <v>95.763999999999996</v>
+      </c>
+      <c r="U50" s="25">
+        <f>278.164-SUM(S50:T50)</f>
+        <v>90.027999999999992</v>
+      </c>
+      <c r="V50" s="25">
+        <f>368.499-SUM(S50:U50)</f>
+        <v>90.335000000000036</v>
+      </c>
+      <c r="W50" s="25">
         <v>85.409000000000006</v>
       </c>
-      <c r="AA50" s="17">
+      <c r="X50" s="25">
+        <f>171.389-W50</f>
+        <v>85.98</v>
+      </c>
+      <c r="Y50" s="25">
+        <f>258.892-SUM(W50:X50)</f>
+        <v>87.502999999999986</v>
+      </c>
+      <c r="Z50" s="25">
+        <f>697.943-SUM(W50:Y50)</f>
+        <v>439.05099999999999</v>
+      </c>
+      <c r="AA50" s="25">
         <v>411.42099999999999</v>
+      </c>
+      <c r="AB50" s="25">
+        <f>826.077-AA50</f>
+        <v>414.65600000000001</v>
       </c>
     </row>
     <row r="51" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="23"/>
-      <c r="M51" s="23"/>
-      <c r="N51" s="23"/>
-      <c r="O51" s="23"/>
-      <c r="P51" s="23"/>
-      <c r="Q51" s="23"/>
-      <c r="R51" s="23"/>
-      <c r="S51" s="23"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="23"/>
-      <c r="V51" s="23"/>
-      <c r="W51" s="23"/>
-      <c r="X51" s="23"/>
-      <c r="Y51" s="23"/>
-      <c r="Z51" s="23"/>
-      <c r="AA51" s="23"/>
-      <c r="AB51" s="23"/>
-      <c r="AC51" s="23"/>
-      <c r="AD51" s="23"/>
-      <c r="AE51" s="23"/>
-      <c r="AF51" s="23"/>
-      <c r="AG51" s="23"/>
-      <c r="AH51" s="23"/>
-      <c r="AI51" s="23"/>
-      <c r="AJ51" s="23"/>
-      <c r="AK51" s="23"/>
-      <c r="AL51" s="23"/>
-      <c r="AM51" s="23"/>
-      <c r="AN51" s="23"/>
-      <c r="AO51" s="23"/>
-      <c r="AP51" s="23"/>
-      <c r="AQ51" s="23"/>
-      <c r="AR51" s="23"/>
-      <c r="AS51" s="23"/>
-      <c r="AT51" s="23"/>
-      <c r="AU51" s="23"/>
-      <c r="AV51" s="23"/>
-      <c r="AW51" s="23"/>
-      <c r="AX51" s="23"/>
-      <c r="AY51" s="23"/>
-      <c r="AZ51" s="23"/>
-      <c r="BA51" s="23"/>
-      <c r="BB51" s="23"/>
-      <c r="BC51" s="23"/>
-      <c r="BD51" s="23"/>
-      <c r="BE51" s="23"/>
-      <c r="BF51" s="23"/>
-      <c r="BG51" s="23"/>
-      <c r="BH51" s="23"/>
-      <c r="BI51" s="23"/>
-      <c r="BJ51" s="23"/>
+      <c r="C51" s="18">
+        <f>C46+SUM(C48:C50)</f>
+        <v>-926.76100000000042</v>
+      </c>
+      <c r="D51" s="18">
+        <f t="shared" ref="D51:AB51" si="104">D46+SUM(D48:D50)</f>
+        <v>-1020.6659999999998</v>
+      </c>
+      <c r="E51" s="18">
+        <f t="shared" si="104"/>
+        <v>-949.79400000000021</v>
+      </c>
+      <c r="F51" s="18">
+        <f t="shared" si="104"/>
+        <v>-310.38599999999957</v>
+      </c>
+      <c r="G51" s="18">
+        <f t="shared" si="104"/>
+        <v>233.94699999999989</v>
+      </c>
+      <c r="H51" s="18">
+        <f t="shared" si="104"/>
+        <v>302.58099999999911</v>
+      </c>
+      <c r="I51" s="18">
+        <f t="shared" si="104"/>
+        <v>518.85599999999943</v>
+      </c>
+      <c r="J51" s="18">
+        <f t="shared" si="104"/>
+        <v>998.375</v>
+      </c>
+      <c r="K51" s="18">
+        <f t="shared" si="104"/>
+        <v>353.17300000000068</v>
+      </c>
+      <c r="L51" s="18">
+        <f t="shared" si="104"/>
+        <v>164.00099999999946</v>
+      </c>
+      <c r="M51" s="18">
+        <f t="shared" si="104"/>
+        <v>1357.1029999999996</v>
+      </c>
+      <c r="N51" s="18">
+        <f t="shared" si="104"/>
+        <v>1365.1830000000002</v>
+      </c>
+      <c r="O51" s="18">
+        <f t="shared" si="104"/>
+        <v>362.44500000000011</v>
+      </c>
+      <c r="P51" s="18">
+        <f t="shared" si="104"/>
+        <v>739.38600000000054</v>
+      </c>
+      <c r="Q51" s="18">
+        <f t="shared" si="104"/>
+        <v>1322.5720000000008</v>
+      </c>
+      <c r="R51" s="18">
+        <f t="shared" si="104"/>
+        <v>1959.8420000000003</v>
+      </c>
+      <c r="S51" s="18">
+        <f t="shared" si="104"/>
+        <v>1532.8240000000005</v>
+      </c>
+      <c r="T51" s="18">
+        <f t="shared" si="104"/>
+        <v>1915.0980000000006</v>
+      </c>
+      <c r="U51" s="18">
+        <f t="shared" si="104"/>
+        <v>1797.5359999999996</v>
+      </c>
+      <c r="V51" s="18">
+        <f t="shared" si="104"/>
+        <v>2437.947000000001</v>
+      </c>
+      <c r="W51" s="18">
+        <f t="shared" si="104"/>
+        <v>895.10100000000057</v>
+      </c>
+      <c r="X51" s="18">
+        <f t="shared" si="104"/>
+        <v>1536.5559999999998</v>
+      </c>
+      <c r="Y51" s="18">
+        <f t="shared" si="104"/>
+        <v>1665.1879999999994</v>
+      </c>
+      <c r="Z51" s="18">
+        <f t="shared" si="104"/>
+        <v>3324.8999999999992</v>
+      </c>
+      <c r="AA51" s="18">
+        <f t="shared" si="104"/>
+        <v>1324.2930000000003</v>
+      </c>
+      <c r="AB51" s="18">
+        <f t="shared" si="104"/>
+        <v>1741.2380000000003</v>
+      </c>
+      <c r="AC51" s="18">
+        <f t="shared" ref="AC51" si="105">AC46+SUM(AC48:AC50)</f>
+        <v>0</v>
+      </c>
+      <c r="AD51" s="18">
+        <f t="shared" ref="AD51" si="106">AD46+SUM(AD48:AD50)</f>
+        <v>0</v>
+      </c>
+      <c r="AE51" s="18">
+        <f t="shared" ref="AE51" si="107">AE46+SUM(AE48:AE50)</f>
+        <v>0</v>
+      </c>
+      <c r="AF51" s="18">
+        <f t="shared" ref="AF51" si="108">AF46+SUM(AF48:AF50)</f>
+        <v>0</v>
+      </c>
+      <c r="AG51" s="18">
+        <f t="shared" ref="AG51" si="109">AG46+SUM(AG48:AG50)</f>
+        <v>0</v>
+      </c>
+      <c r="AH51" s="18">
+        <f t="shared" ref="AH51" si="110">AH46+SUM(AH48:AH50)</f>
+        <v>0</v>
+      </c>
+      <c r="AI51" s="18">
+        <f t="shared" ref="AI51" si="111">AI46+SUM(AI48:AI50)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="18">
+        <f t="shared" ref="AJ51" si="112">AJ46+SUM(AJ48:AJ50)</f>
+        <v>0</v>
+      </c>
+      <c r="AK51" s="18">
+        <f t="shared" ref="AK51" si="113">AK46+SUM(AK48:AK50)</f>
+        <v>0</v>
+      </c>
+      <c r="AL51" s="18">
+        <f t="shared" ref="AL51" si="114">AL46+SUM(AL48:AL50)</f>
+        <v>0</v>
+      </c>
+      <c r="AM51" s="18">
+        <f t="shared" ref="AM51" si="115">AM46+SUM(AM48:AM50)</f>
+        <v>0</v>
+      </c>
+      <c r="AN51" s="18">
+        <f t="shared" ref="AN51" si="116">AN46+SUM(AN48:AN50)</f>
+        <v>0</v>
+      </c>
+      <c r="AO51" s="18">
+        <f t="shared" ref="AO51" si="117">AO46+SUM(AO48:AO50)</f>
+        <v>0</v>
+      </c>
+      <c r="AP51" s="18">
+        <f t="shared" ref="AP51" si="118">AP46+SUM(AP48:AP50)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ51" s="18">
+        <f t="shared" ref="AQ51" si="119">AQ46+SUM(AQ48:AQ50)</f>
+        <v>0</v>
+      </c>
+      <c r="AR51" s="18">
+        <f t="shared" ref="AR51" si="120">AR46+SUM(AR48:AR50)</f>
+        <v>0</v>
+      </c>
+      <c r="AS51" s="18">
+        <f t="shared" ref="AS51" si="121">AS46+SUM(AS48:AS50)</f>
+        <v>0</v>
+      </c>
+      <c r="AT51" s="18">
+        <f t="shared" ref="AT51" si="122">AT46+SUM(AT48:AT50)</f>
+        <v>0</v>
+      </c>
+      <c r="AU51" s="18">
+        <f t="shared" ref="AU51" si="123">AU46+SUM(AU48:AU50)</f>
+        <v>0</v>
+      </c>
+      <c r="AV51" s="18">
+        <f t="shared" ref="AV51" si="124">AV46+SUM(AV48:AV50)</f>
+        <v>0</v>
+      </c>
+      <c r="AW51" s="18">
+        <f t="shared" ref="AW51" si="125">AW46+SUM(AW48:AW50)</f>
+        <v>0</v>
+      </c>
+      <c r="AX51" s="18">
+        <f t="shared" ref="AX51" si="126">AX46+SUM(AX48:AX50)</f>
+        <v>0</v>
+      </c>
+      <c r="AY51" s="18">
+        <f t="shared" ref="AY51" si="127">AY46+SUM(AY48:AY50)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ51" s="18">
+        <f t="shared" ref="AZ51" si="128">AZ46+SUM(AZ48:AZ50)</f>
+        <v>0</v>
+      </c>
+      <c r="BA51" s="18">
+        <f t="shared" ref="BA51" si="129">BA46+SUM(BA48:BA50)</f>
+        <v>0</v>
+      </c>
+      <c r="BB51" s="18">
+        <f t="shared" ref="BB51" si="130">BB46+SUM(BB48:BB50)</f>
+        <v>0</v>
+      </c>
+      <c r="BC51" s="18">
+        <f t="shared" ref="BC51" si="131">BC46+SUM(BC48:BC50)</f>
+        <v>0</v>
+      </c>
+      <c r="BD51" s="18">
+        <f t="shared" ref="BD51" si="132">BD46+SUM(BD48:BD50)</f>
+        <v>0</v>
+      </c>
+      <c r="BE51" s="18">
+        <f t="shared" ref="BE51" si="133">BE46+SUM(BE48:BE50)</f>
+        <v>0</v>
+      </c>
+      <c r="BF51" s="18">
+        <f t="shared" ref="BF51" si="134">BF46+SUM(BF48:BF50)</f>
+        <v>0</v>
+      </c>
+      <c r="BG51" s="18">
+        <f t="shared" ref="BG51" si="135">BG46+SUM(BG48:BG50)</f>
+        <v>0</v>
+      </c>
+      <c r="BH51" s="18">
+        <f t="shared" ref="BH51" si="136">BH46+SUM(BH48:BH50)</f>
+        <v>0</v>
+      </c>
+      <c r="BI51" s="18">
+        <f t="shared" ref="BI51" si="137">BI46+SUM(BI48:BI50)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ51" s="18">
+        <f t="shared" ref="BJ51" si="138">BJ46+SUM(BJ48:BJ50)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:62" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="23"/>
-      <c r="M52" s="23"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="23"/>
-      <c r="P52" s="23"/>
-      <c r="Q52" s="23"/>
-      <c r="R52" s="23"/>
-      <c r="S52" s="23"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="23"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="23"/>
-      <c r="X52" s="23"/>
-      <c r="Y52" s="23"/>
-      <c r="Z52" s="23"/>
-      <c r="AA52" s="23"/>
-      <c r="AB52" s="23"/>
-      <c r="AC52" s="23"/>
-      <c r="AD52" s="23"/>
-      <c r="AE52" s="23"/>
-      <c r="AF52" s="23"/>
-      <c r="AG52" s="23"/>
-      <c r="AH52" s="23"/>
-      <c r="AI52" s="23"/>
-      <c r="AJ52" s="23"/>
-      <c r="AK52" s="23"/>
-      <c r="AL52" s="23"/>
-      <c r="AM52" s="23"/>
-      <c r="AN52" s="23"/>
-      <c r="AO52" s="23"/>
-      <c r="AP52" s="23"/>
-      <c r="AQ52" s="23"/>
-      <c r="AR52" s="23"/>
-      <c r="AS52" s="23"/>
-      <c r="AT52" s="23"/>
-      <c r="AU52" s="23"/>
-      <c r="AV52" s="23"/>
-      <c r="AW52" s="23"/>
-      <c r="AX52" s="23"/>
-      <c r="AY52" s="23"/>
-      <c r="AZ52" s="23"/>
-      <c r="BA52" s="23"/>
-      <c r="BB52" s="23"/>
-      <c r="BC52" s="23"/>
-      <c r="BD52" s="23"/>
-      <c r="BE52" s="23"/>
-      <c r="BF52" s="23"/>
-      <c r="BG52" s="23"/>
-      <c r="BH52" s="23"/>
-      <c r="BI52" s="23"/>
-      <c r="BJ52" s="23"/>
+      <c r="C52" s="11">
+        <f>C51/C18</f>
+        <v>-0.30011845916300101</v>
+      </c>
+      <c r="D52" s="11">
+        <f t="shared" ref="D52:AB52" si="139">D51/D18</f>
+        <v>-0.27384226889647034</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="139"/>
+        <v>-0.28020307623501223</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="139"/>
+        <v>-8.5141739685493392E-2</v>
+      </c>
+      <c r="G52" s="11">
+        <f t="shared" si="139"/>
+        <v>5.8815380941007855E-2</v>
+      </c>
+      <c r="H52" s="11">
+        <f t="shared" si="139"/>
+        <v>7.1989497343287301E-2</v>
+      </c>
+      <c r="I52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.11304485749344625</v>
+      </c>
+      <c r="J52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.2079086828205319</v>
+      </c>
+      <c r="K52" s="11">
+        <f t="shared" si="139"/>
+        <v>7.8284082113246764E-2</v>
+      </c>
+      <c r="L52" s="11">
+        <f t="shared" si="139"/>
+        <v>3.3919088988462298E-2</v>
+      </c>
+      <c r="M52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.22794321302305171</v>
+      </c>
+      <c r="N52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.21686724595024925</v>
+      </c>
+      <c r="O52" s="11">
+        <f t="shared" si="139"/>
+        <v>7.4429343205633602E-2</v>
+      </c>
+      <c r="P52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.14435930802279268</v>
+      </c>
+      <c r="Q52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.21400207728476658</v>
+      </c>
+      <c r="R52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.28514606766421524</v>
+      </c>
+      <c r="S52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.22892395775367708</v>
+      </c>
+      <c r="T52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.2797470573284136</v>
+      </c>
+      <c r="U52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.2591612197043357</v>
+      </c>
+      <c r="V52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.3356610746261835</v>
+      </c>
+      <c r="W52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.13736430858456153</v>
+      </c>
+      <c r="X52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.20932710701545162</v>
+      </c>
+      <c r="Y52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.20921528875737377</v>
+      </c>
+      <c r="Z52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.25590730720075544</v>
+      </c>
+      <c r="AA52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.14227374696539982</v>
+      </c>
+      <c r="AB52" s="11">
+        <f t="shared" si="139"/>
+        <v>0.16213374978909667</v>
+      </c>
+      <c r="AC52" s="11" t="e">
+        <f t="shared" ref="AC52" si="140">AC51/AC18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD52" s="11" t="e">
+        <f t="shared" ref="AD52" si="141">AD51/AD18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE52" s="11" t="e">
+        <f t="shared" ref="AE52" si="142">AE51/AE18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF52" s="11" t="e">
+        <f t="shared" ref="AF52" si="143">AF51/AF18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AG52" s="11" t="e">
+        <f t="shared" ref="AG52" si="144">AG51/AG18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AH52" s="11" t="e">
+        <f t="shared" ref="AH52" si="145">AH51/AH18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI52" s="11" t="e">
+        <f t="shared" ref="AI52" si="146">AI51/AI18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ52" s="11" t="e">
+        <f t="shared" ref="AJ52" si="147">AJ51/AJ18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK52" s="11" t="e">
+        <f t="shared" ref="AK52" si="148">AK51/AK18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AL52" s="11" t="e">
+        <f t="shared" ref="AL52" si="149">AL51/AL18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM52" s="11" t="e">
+        <f t="shared" ref="AM52" si="150">AM51/AM18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN52" s="11" t="e">
+        <f t="shared" ref="AN52" si="151">AN51/AN18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO52" s="11" t="e">
+        <f t="shared" ref="AO52" si="152">AO51/AO18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AP52" s="11" t="e">
+        <f t="shared" ref="AP52" si="153">AP51/AP18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AQ52" s="11" t="e">
+        <f t="shared" ref="AQ52" si="154">AQ51/AQ18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR52" s="11" t="e">
+        <f t="shared" ref="AR52" si="155">AR51/AR18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS52" s="11" t="e">
+        <f t="shared" ref="AS52" si="156">AS51/AS18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AT52" s="11" t="e">
+        <f t="shared" ref="AT52" si="157">AT51/AT18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU52" s="11" t="e">
+        <f t="shared" ref="AU52" si="158">AU51/AU18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AV52" s="11" t="e">
+        <f t="shared" ref="AV52" si="159">AV51/AV18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AW52" s="11" t="e">
+        <f t="shared" ref="AW52" si="160">AW51/AW18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AX52" s="11" t="e">
+        <f t="shared" ref="AX52" si="161">AX51/AX18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AY52" s="11" t="e">
+        <f t="shared" ref="AY52" si="162">AY51/AY18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AZ52" s="11" t="e">
+        <f t="shared" ref="AZ52" si="163">AZ51/AZ18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BA52" s="11" t="e">
+        <f t="shared" ref="BA52" si="164">BA51/BA18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BB52" s="11" t="e">
+        <f t="shared" ref="BB52" si="165">BB51/BB18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC52" s="11" t="e">
+        <f t="shared" ref="BC52" si="166">BC51/BC18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BD52" s="11" t="e">
+        <f t="shared" ref="BD52" si="167">BD51/BD18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BE52" s="11" t="e">
+        <f t="shared" ref="BE52" si="168">BE51/BE18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BF52" s="11" t="e">
+        <f t="shared" ref="BF52" si="169">BF51/BF18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BG52" s="11" t="e">
+        <f t="shared" ref="BG52" si="170">BG51/BG18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BH52" s="11" t="e">
+        <f t="shared" ref="BH52" si="171">BH51/BH18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BI52" s="11" t="e">
+        <f t="shared" ref="BI52" si="172">BI51/BI18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BJ52" s="11" t="e">
+        <f t="shared" ref="BJ52" si="173">BJ51/BJ18</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="54" spans="1:62" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
@@ -6358,239 +6790,239 @@
         <v>-5.2530073504171985E-2</v>
       </c>
       <c r="D59" s="20">
-        <f t="shared" ref="D59:BJ59" si="103">D$46/D55</f>
+        <f t="shared" ref="D59:BJ59" si="174">D$46/D55</f>
         <v>-7.8384040136559918E-2</v>
       </c>
       <c r="E59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>-6.1904443629652632E-2</v>
       </c>
       <c r="F59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>-2.4630531330878922E-2</v>
       </c>
       <c r="G59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>8.2788622898745997E-3</v>
       </c>
       <c r="H59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>1.2010212230098008E-2</v>
       </c>
       <c r="I59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>3.0287243604853683E-2</v>
       </c>
       <c r="J59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>5.9040510656479493E-2</v>
       </c>
       <c r="K59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>1.9392471575552898E-2</v>
       </c>
       <c r="L59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>2.5875697191765815E-2</v>
       </c>
       <c r="M59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>7.4314870907893224E-2</v>
       </c>
       <c r="N59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>7.3326259947575065E-2</v>
       </c>
       <c r="O59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>1.3950252300634174E-2</v>
       </c>
       <c r="P59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>3.5336846441780145E-2</v>
       </c>
       <c r="Q59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>0.15588280170375748</v>
       </c>
       <c r="R59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>8.8837237843157779E-2</v>
       </c>
       <c r="S59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>6.5698339337687983E-2</v>
       </c>
       <c r="T59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>8.2855630307760456E-2</v>
       </c>
       <c r="U59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>7.8740890992934548E-2</v>
       </c>
       <c r="V59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>9.5694496356498251E-2</v>
       </c>
       <c r="W59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>4.034535085823765E-2</v>
       </c>
       <c r="X59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>7.3252541155832573E-2</v>
       </c>
       <c r="Y59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>8.0979775295729278E-2</v>
       </c>
       <c r="Z59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>0.15140926559160772</v>
       </c>
       <c r="AA59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>6.0588394189519439E-2</v>
       </c>
       <c r="AB59" s="20">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>6.9220193261732871E-2</v>
       </c>
       <c r="AC59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AL59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AM59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AN59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AO59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AP59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AQ59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AS59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AT59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AU59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AV59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AW59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AX59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AY59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AZ59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BA59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BB59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BC59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BD59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BE59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BF59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BG59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BH59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BI59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BJ59" s="20" t="e">
-        <f t="shared" si="103"/>
+        <f t="shared" si="174"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6603,239 +7035,239 @@
         <v>-5.2530073504171985E-2</v>
       </c>
       <c r="D60" s="20">
-        <f t="shared" ref="D60:BJ60" si="104">D$46/D56</f>
+        <f t="shared" ref="D60:BJ60" si="175">D$46/D56</f>
         <v>-7.8384040136559918E-2</v>
       </c>
       <c r="E60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>-6.1904443629652632E-2</v>
       </c>
       <c r="F60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>-2.4630531330878922E-2</v>
       </c>
       <c r="G60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>8.2788622898745997E-3</v>
       </c>
       <c r="H60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>1.1999428765113375E-2</v>
       </c>
       <c r="I60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>3.011188821156081E-2</v>
       </c>
       <c r="J60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>5.8396908899505551E-2</v>
       </c>
       <c r="K60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>1.9196587106882084E-2</v>
       </c>
       <c r="L60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>2.5585182091301058E-2</v>
       </c>
       <c r="M60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>7.3730773338639394E-2</v>
       </c>
       <c r="N60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>7.2469876096192598E-2</v>
       </c>
       <c r="O60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>1.3948710311346464E-2</v>
       </c>
       <c r="P60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>3.5333085849173961E-2</v>
       </c>
       <c r="Q60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>0.15587329391777988</v>
       </c>
       <c r="R60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>8.8831064944835392E-2</v>
       </c>
       <c r="S60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>6.5698339337687983E-2</v>
       </c>
       <c r="T60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>8.2855630307760456E-2</v>
       </c>
       <c r="U60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>7.8720601271948146E-2</v>
       </c>
       <c r="V60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>9.568828043737268E-2</v>
       </c>
       <c r="W60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>4.0323436612704613E-2</v>
       </c>
       <c r="X60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>7.3245407550868585E-2</v>
       </c>
       <c r="Y60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>8.097692356880816E-2</v>
       </c>
       <c r="Z60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>0.15096977797774996</v>
       </c>
       <c r="AA60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>6.0506763240958231E-2</v>
       </c>
       <c r="AB60" s="20">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>6.9095876163622241E-2</v>
       </c>
       <c r="AC60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AH60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AI60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AK60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AL60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AM60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AN60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AO60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AP60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AQ60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AR60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AS60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AT60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AU60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AV60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AW60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AX60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AY60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AZ60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BA60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BB60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BC60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BD60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BE60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BF60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BG60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BH60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BI60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BJ60" s="20" t="e">
-        <f t="shared" si="104"/>
+        <f t="shared" si="175"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>